<commit_message>
nota contabila nr automat + sold clienti dar dif pe CN
</commit_message>
<xml_diff>
--- a/website/static/Template_NC.xlsx
+++ b/website/static/Template_NC.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\35. GIT RAS\RAS_Expeditors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\35. GIT RAS\RAS_Expeditors\website\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{587C6C84-8852-45C4-9A6F-9BBA55F7BB5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1057BDF5-BB29-4158-856D-4328551C25D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{769C8F87-AF0D-4F73-A1CC-FC9863B7C3BD}"/>
   </bookViews>
@@ -20,13 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
-  <si>
-    <t>JT</t>
-  </si>
-  <si>
-    <t>GL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>BR</t>
   </si>
@@ -34,112 +28,46 @@
     <t>Statutory_GL</t>
   </si>
   <si>
-    <t>Prod</t>
-  </si>
-  <si>
-    <t>GL_Type</t>
-  </si>
-  <si>
-    <t>GL_Group</t>
-  </si>
-  <si>
-    <t>GL_Subtype</t>
-  </si>
-  <si>
-    <t>GL_Cat</t>
-  </si>
-  <si>
     <t>Journal</t>
   </si>
   <si>
+    <t>Open_Item</t>
+  </si>
+  <si>
+    <t>File_Ref</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>data_Description</t>
+  </si>
+  <si>
+    <t>Post_Date</t>
+  </si>
+  <si>
+    <t>Foreign Amount</t>
+  </si>
+  <si>
+    <t>Foreign Currency</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
     <t>GCI</t>
-  </si>
-  <si>
-    <t>GCI_Br</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Open_Item</t>
-  </si>
-  <si>
-    <t>File_Ref</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>TC</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>Foreign_Amount</t>
-  </si>
-  <si>
-    <t>Foreign_Currency</t>
-  </si>
-  <si>
-    <t>External_Ref</t>
-  </si>
-  <si>
-    <t>MBL</t>
-  </si>
-  <si>
-    <t>IC</t>
-  </si>
-  <si>
-    <t>House</t>
-  </si>
-  <si>
-    <t>BC</t>
-  </si>
-  <si>
-    <t>Billing_Description</t>
-  </si>
-  <si>
-    <t>Customer_GCI</t>
-  </si>
-  <si>
-    <t>Customer_Name</t>
-  </si>
-  <si>
-    <t>data_Description</t>
-  </si>
-  <si>
-    <t>GL_Description</t>
-  </si>
-  <si>
-    <t>GL_Local_Description</t>
-  </si>
-  <si>
-    <t>Post_Date</t>
-  </si>
-  <si>
-    <t>Last_Modifier</t>
-  </si>
-  <si>
-    <t>Approver</t>
-  </si>
-  <si>
-    <t>Acct_Tran_Id</t>
-  </si>
-  <si>
-    <t>RowNumber</t>
-  </si>
-  <si>
-    <t>Commissionable</t>
-  </si>
-  <si>
-    <t>data_Source</t>
   </si>
 </sst>
 </file>
@@ -1000,15 +928,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5AD134-8B17-4391-8983-4C7F167D9B7F}">
-  <dimension ref="A1:AN1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1034,16 +962,16 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
       </c>
       <c r="M1" t="s">
         <v>12</v>
@@ -1052,82 +980,10 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
         <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>